<commit_message>
Add averages notebook, add optimization to rigorous method
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaysh\source\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHAHJ\source\repos\jay-r-shah\pwlf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDB82B8-1B68-4A2B-B8B6-8480670CCE78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D3552-8130-4B83-BCCB-DF7416EEF60E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{D0C2CEFF-9B5B-4B0C-A8F7-24A53073BF2C}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{D0C2CEFF-9B5B-4B0C-A8F7-24A53073BF2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -4427,17 +4427,17 @@
   <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A122"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>5</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>103.93550071329705</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>7</v>
       </c>
@@ -4478,459 +4478,459 @@
         <v>9.2940596273242697</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">B3+C3</f>
+        <f>B3+C3</f>
         <v>112.6273929606576</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>9</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B31" si="1">B3+($B$32-$B$2)/30</f>
+        <f t="shared" ref="B4:B31" si="0">B3+($B$32-$B$2)/30</f>
         <v>106.66666666666666</v>
       </c>
       <c r="C4" s="2">
         <v>-5.5608612560271302</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>B4+C4</f>
         <v>101.10580541063953</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>11</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>109.99999999999999</v>
       </c>
       <c r="C5" s="2">
         <v>-3.0899800798177899</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>B5+C5</f>
         <v>106.91001992018219</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>13</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>113.33333333333331</v>
       </c>
       <c r="C6" s="2">
         <v>7.7388440825571001</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>B6+C6</f>
         <v>121.07217741589041</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>15</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>116.66666666666664</v>
       </c>
       <c r="C7" s="2">
         <v>-5.3592848270678797</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>B7+C7</f>
         <v>111.30738183959876</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>17</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>119.99999999999997</v>
       </c>
       <c r="C8" s="2">
         <v>-5.4140749631350902</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>B8+C8</f>
         <v>114.58592503686488</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>19</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>123.3333333333333</v>
       </c>
       <c r="C9" s="2">
         <v>-8.0943692022431293</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>B9+C9</f>
         <v>115.23896413109017</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>21</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>126.66666666666663</v>
       </c>
       <c r="C10" s="2">
         <v>4.7429808416462702</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>B10+C10</f>
         <v>131.4096475083129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>23</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>129.99999999999997</v>
       </c>
       <c r="C11" s="2">
         <v>-7.8256443569850198</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>B11+C11</f>
         <v>122.17435564301495</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>25</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>133.33333333333331</v>
       </c>
       <c r="C12" s="2">
         <v>2.4646947207260301</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f>B12+C12</f>
         <v>135.79802805405936</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>27</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>136.66666666666666</v>
       </c>
       <c r="C13" s="2">
         <v>-2.7910179830253301</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>B13+C13</f>
         <v>133.87564868364132</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>29</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="C14" s="2">
         <v>5.5910325525942604</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>B14+C14</f>
         <v>145.59103255259427</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>31</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>143.33333333333334</v>
       </c>
       <c r="C15" s="2">
         <v>16.266769240242699</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>B15+C15</f>
         <v>159.60010257357604</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>33</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>146.66666666666669</v>
       </c>
       <c r="C16" s="2">
         <v>-7.4570117814422696</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f>B16+C16</f>
         <v>139.20965488522441</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>35</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>150.00000000000003</v>
       </c>
       <c r="C17" s="2">
         <v>-3.65667121959416</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f>B17+C17</f>
         <v>146.34332878040587</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>37</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>153.33333333333337</v>
       </c>
       <c r="C18" s="2">
         <v>-4.4878917061276402</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>B18+C18</f>
         <v>148.84544162720573</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>39</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>156.66666666666671</v>
       </c>
       <c r="C19" s="2">
         <v>-8.02736427062346</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>B19+C19</f>
         <v>148.63930239604326</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>41</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>160.00000000000006</v>
       </c>
       <c r="C20" s="2">
         <v>2.4721368296225799</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f>B20+C20</f>
         <v>162.47213682962263</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>163.3333333333334</v>
       </c>
       <c r="C21" s="2">
         <v>4.6569310449723904</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>B21+C21</f>
         <v>167.9902643783058</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>166.66666666666674</v>
       </c>
       <c r="C22" s="2">
         <v>-2.9977630263056398</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>B22+C22</f>
         <v>163.66890364036109</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>47</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>170.00000000000009</v>
       </c>
       <c r="C23" s="2">
         <v>0.455968814310173</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>B23+C23</f>
         <v>170.45596881431027</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>49</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>173.33333333333343</v>
       </c>
       <c r="C24" s="2">
         <v>-1.01607020055855</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f>B24+C24</f>
         <v>172.31726313277488</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>51</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>176.66666666666677</v>
       </c>
       <c r="C25" s="2">
         <v>2.7147492197386902</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f>B25+C25</f>
         <v>179.38141588640545</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>53</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>180.00000000000011</v>
       </c>
       <c r="C26" s="2">
         <v>-4.1772409341537404</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f>B26+C26</f>
         <v>175.82275906584638</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>55</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>183.33333333333346</v>
       </c>
       <c r="C27" s="2">
         <v>9.5710999974831701</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f>B27+C27</f>
         <v>192.90443333081663</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>57</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>186.6666666666668</v>
       </c>
       <c r="C28" s="2">
         <v>5.5197920913799301</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>B28+C28</f>
         <v>192.18645875804674</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>59</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>190.00000000000014</v>
       </c>
       <c r="C29" s="2">
         <v>3.2091132501812498</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>B29+C29</f>
         <v>193.20911325018139</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>61</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>193.33333333333348</v>
       </c>
       <c r="C30" s="2">
         <v>-2.8529473385148298</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f>B30+C30</f>
         <v>190.48038599481865</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>63</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>196.66666666666683</v>
       </c>
       <c r="C31" s="2">
         <v>8.1511721719512398</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f>B31+C31</f>
         <v>204.81783883861806</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>65</v>
       </c>
@@ -4941,11 +4941,11 @@
         <v>-6.3517945600520003</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f>B32+C32</f>
         <v>193.64820543994799</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>67</v>
       </c>
@@ -4957,459 +4957,459 @@
         <v>-4.62377634796945</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f>B33+C33</f>
         <v>195.37622365203055</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>69</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:B61" si="2">B33+($B$62-$B$32)/30</f>
+        <f t="shared" ref="B34:B61" si="1">B33+($B$62-$B$32)/30</f>
         <v>200</v>
       </c>
       <c r="C34" s="2">
         <v>-4.7944027539971099</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f>B34+C34</f>
         <v>195.2055972460029</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>71</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C35" s="2">
         <v>1.21117661501559</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f>B35+C35</f>
         <v>201.2111766150156</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>73</v>
       </c>
       <c r="B36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C36" s="2">
         <v>-4.7829096453378703</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f>B36+C36</f>
         <v>195.21709035466213</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>75</v>
       </c>
       <c r="B37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C37" s="2">
         <v>2.3914523600752</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
+        <f>B37+C37</f>
         <v>202.39145236007519</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>77</v>
       </c>
       <c r="B38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C38" s="2">
         <v>-4.7857653460447001</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
+        <f>B38+C38</f>
         <v>195.21423465395529</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>79</v>
       </c>
       <c r="B39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C39" s="2">
         <v>0.77219147691683199</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
+        <f>B39+C39</f>
         <v>200.77219147691684</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>81</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C40" s="2">
         <v>-1.9732941791927701</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
+        <f>B40+C40</f>
         <v>198.02670582080722</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>83</v>
       </c>
       <c r="B41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C41" s="2">
         <v>-3.1004790756897802</v>
       </c>
       <c r="D41">
-        <f t="shared" si="0"/>
+        <f>B41+C41</f>
         <v>196.89952092431022</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>85</v>
       </c>
       <c r="B42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C42" s="2">
         <v>3.6098986396367199</v>
       </c>
       <c r="D42">
-        <f t="shared" si="0"/>
+        <f>B42+C42</f>
         <v>203.60989863963673</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>87</v>
       </c>
       <c r="B43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C43" s="2">
         <v>-4.7811372635988798</v>
       </c>
       <c r="D43">
-        <f t="shared" si="0"/>
+        <f>B43+C43</f>
         <v>195.21886273640112</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>89</v>
       </c>
       <c r="B44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C44" s="2">
         <v>-3.11194754155547</v>
       </c>
       <c r="D44">
-        <f t="shared" si="0"/>
+        <f>B44+C44</f>
         <v>196.88805245844452</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>91</v>
       </c>
       <c r="B45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C45" s="2">
         <v>-5.8859848836223902E-2</v>
       </c>
       <c r="D45">
-        <f t="shared" si="0"/>
+        <f>B45+C45</f>
         <v>199.94114015116378</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>93</v>
       </c>
       <c r="B46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C46" s="2">
         <v>10.098417600050301</v>
       </c>
       <c r="D46">
-        <f t="shared" si="0"/>
+        <f>B46+C46</f>
         <v>210.09841760005031</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>95</v>
       </c>
       <c r="B47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C47" s="2">
         <v>7.4824475617088897</v>
       </c>
       <c r="D47">
-        <f t="shared" si="0"/>
+        <f>B47+C47</f>
         <v>207.48244756170888</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>97</v>
       </c>
       <c r="B48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C48" s="2">
         <v>0.49883097426723499</v>
       </c>
       <c r="D48">
-        <f t="shared" si="0"/>
+        <f>B48+C48</f>
         <v>200.49883097426724</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>99</v>
       </c>
       <c r="B49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C49" s="2">
         <v>1.50902649532342</v>
       </c>
       <c r="D49">
-        <f t="shared" si="0"/>
+        <f>B49+C49</f>
         <v>201.50902649532341</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>101</v>
       </c>
       <c r="B50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C50" s="2">
         <v>4.1434391281909297</v>
       </c>
       <c r="D50">
-        <f t="shared" si="0"/>
+        <f>B50+C50</f>
         <v>204.14343912819092</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>103</v>
       </c>
       <c r="B51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C51" s="2">
         <v>-1.7042752112723201</v>
       </c>
       <c r="D51">
-        <f t="shared" si="0"/>
+        <f>B51+C51</f>
         <v>198.29572478872768</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>105</v>
       </c>
       <c r="B52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C52" s="2">
         <v>4.4631503833291299</v>
       </c>
       <c r="D52">
-        <f t="shared" si="0"/>
+        <f>B52+C52</f>
         <v>204.46315038332912</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>107</v>
       </c>
       <c r="B53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C53" s="2">
         <v>-0.767012215525403</v>
       </c>
       <c r="D53">
-        <f t="shared" si="0"/>
+        <f>B53+C53</f>
         <v>199.2329877844746</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>109</v>
       </c>
       <c r="B54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C54" s="2">
         <v>1.5182688499718999</v>
       </c>
       <c r="D54">
-        <f t="shared" si="0"/>
+        <f>B54+C54</f>
         <v>201.51826884997189</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>111</v>
       </c>
       <c r="B55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C55" s="2">
         <v>-2.66750594875018</v>
       </c>
       <c r="D55">
-        <f t="shared" si="0"/>
+        <f>B55+C55</f>
         <v>197.33249405124982</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>113</v>
       </c>
       <c r="B56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C56" s="2">
         <v>2.4033322185630501</v>
       </c>
       <c r="D56">
-        <f t="shared" si="0"/>
+        <f>B56+C56</f>
         <v>202.40333221856304</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>115</v>
       </c>
       <c r="B57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C57" s="2">
         <v>-10.797540050142</v>
       </c>
       <c r="D57">
-        <f t="shared" si="0"/>
+        <f>B57+C57</f>
         <v>189.202459949858</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>117</v>
       </c>
       <c r="B58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C58" s="2">
         <v>-1.1272653538742301</v>
       </c>
       <c r="D58">
-        <f t="shared" si="0"/>
+        <f>B58+C58</f>
         <v>198.87273464612576</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>119</v>
       </c>
       <c r="B59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C59" s="2">
         <v>2.2432469212422599</v>
       </c>
       <c r="D59">
-        <f t="shared" si="0"/>
+        <f>B59+C59</f>
         <v>202.24324692124225</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>121</v>
       </c>
       <c r="B60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C60" s="2">
         <v>2.6217160678765299</v>
       </c>
       <c r="D60">
-        <f t="shared" si="0"/>
+        <f>B60+C60</f>
         <v>202.62171606787652</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>123</v>
       </c>
       <c r="B61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="C61" s="2">
         <v>5.1903828175833802</v>
       </c>
       <c r="D61">
-        <f t="shared" si="0"/>
+        <f>B61+C61</f>
         <v>205.19038281758338</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>125</v>
       </c>
@@ -5420,11 +5420,11 @@
         <v>4.5485251254126204</v>
       </c>
       <c r="D62">
-        <f t="shared" si="0"/>
+        <f>B62+C62</f>
         <v>204.54852512541262</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>127</v>
       </c>
@@ -5436,459 +5436,459 @@
         <v>2.70336013228528</v>
       </c>
       <c r="D63">
-        <f t="shared" si="0"/>
+        <f>B63+C63</f>
         <v>201.03669346561861</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>129</v>
       </c>
       <c r="B64">
-        <f t="shared" ref="B64:B91" si="3">B63+($B$92-$B$62)/30</f>
+        <f t="shared" ref="B64:B91" si="2">B63+($B$92-$B$62)/30</f>
         <v>196.66666666666669</v>
       </c>
       <c r="C64" s="2">
         <v>-3.8393747958240501</v>
       </c>
       <c r="D64">
-        <f t="shared" si="0"/>
+        <f>B64+C64</f>
         <v>192.82729187084263</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>131</v>
       </c>
       <c r="B65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>195.00000000000003</v>
       </c>
       <c r="C65" s="2">
         <v>-0.95172812158366604</v>
       </c>
       <c r="D65">
-        <f t="shared" si="0"/>
+        <f>B65+C65</f>
         <v>194.04827187841636</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>133</v>
       </c>
       <c r="B66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>193.33333333333337</v>
       </c>
       <c r="C66" s="2">
         <v>0.54360743619514895</v>
       </c>
       <c r="D66">
-        <f t="shared" si="0"/>
+        <f>B66+C66</f>
         <v>193.87694076952852</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>135</v>
       </c>
       <c r="B67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>191.66666666666671</v>
       </c>
       <c r="C67" s="2">
         <v>1.6252795962420199</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D122" si="4">B67+C67</f>
+        <f>B67+C67</f>
         <v>193.29194626290874</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>137</v>
       </c>
       <c r="B68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>190.00000000000006</v>
       </c>
       <c r="C68" s="2">
         <v>-3.87818462412858</v>
       </c>
       <c r="D68">
-        <f t="shared" si="4"/>
+        <f>B68+C68</f>
         <v>186.12181537587148</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>139</v>
       </c>
       <c r="B69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>188.3333333333334</v>
       </c>
       <c r="C69" s="2">
         <v>-6.4435259666172504</v>
       </c>
       <c r="D69">
-        <f t="shared" si="4"/>
+        <f>B69+C69</f>
         <v>181.88980736671616</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>141</v>
       </c>
       <c r="B70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>186.66666666666674</v>
       </c>
       <c r="C70" s="2">
         <v>2.7751700106266899</v>
       </c>
       <c r="D70">
-        <f t="shared" si="4"/>
+        <f>B70+C70</f>
         <v>189.44183667729342</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>143</v>
       </c>
       <c r="B71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>185.00000000000009</v>
       </c>
       <c r="C71" s="2">
         <v>-5.1470094769702497</v>
       </c>
       <c r="D71">
-        <f t="shared" si="4"/>
+        <f>B71+C71</f>
         <v>179.85299052302983</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>145</v>
       </c>
       <c r="B72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>183.33333333333343</v>
       </c>
       <c r="C72" s="2">
         <v>7.3824685932197198</v>
       </c>
       <c r="D72">
-        <f t="shared" si="4"/>
+        <f>B72+C72</f>
         <v>190.71580192655315</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>147</v>
       </c>
       <c r="B73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>181.66666666666677</v>
       </c>
       <c r="C73" s="2">
         <v>8.8047834262010198</v>
       </c>
       <c r="D73">
-        <f t="shared" si="4"/>
+        <f>B73+C73</f>
         <v>190.4714500928678</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>149</v>
       </c>
       <c r="B74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>180.00000000000011</v>
       </c>
       <c r="C74" s="2">
         <v>-4.1219355255746501</v>
       </c>
       <c r="D74">
-        <f t="shared" si="4"/>
+        <f>B74+C74</f>
         <v>175.87806447442546</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>151</v>
       </c>
       <c r="B75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>178.33333333333346</v>
       </c>
       <c r="C75" s="2">
         <v>-0.52461088066200101</v>
       </c>
       <c r="D75">
-        <f t="shared" si="4"/>
+        <f>B75+C75</f>
         <v>177.80872245267145</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>153</v>
       </c>
       <c r="B76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>176.6666666666668</v>
       </c>
       <c r="C76" s="2">
         <v>-2.1872483700549199</v>
       </c>
       <c r="D76">
-        <f t="shared" si="4"/>
+        <f>B76+C76</f>
         <v>174.47941829661187</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>155</v>
       </c>
       <c r="B77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>175.00000000000014</v>
       </c>
       <c r="C77" s="2">
         <v>5.6199142849594701E-2</v>
       </c>
       <c r="D77">
-        <f t="shared" si="4"/>
+        <f>B77+C77</f>
         <v>175.05619914284975</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>157</v>
       </c>
       <c r="B78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>173.33333333333348</v>
       </c>
       <c r="C78" s="2">
         <v>3.62863001589773</v>
       </c>
       <c r="D78">
-        <f t="shared" si="4"/>
+        <f>B78+C78</f>
         <v>176.96196334923121</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>159</v>
       </c>
       <c r="B79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>171.66666666666683</v>
       </c>
       <c r="C79" s="2">
         <v>-2.46123645181066</v>
       </c>
       <c r="D79">
-        <f t="shared" si="4"/>
+        <f>B79+C79</f>
         <v>169.20543021485616</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>161</v>
       </c>
       <c r="B80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>170.00000000000017</v>
       </c>
       <c r="C80" s="2">
         <v>9.0495615626642198</v>
       </c>
       <c r="D80">
-        <f t="shared" si="4"/>
+        <f>B80+C80</f>
         <v>179.04956156266439</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>163</v>
       </c>
       <c r="B81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>168.33333333333351</v>
       </c>
       <c r="C81" s="2">
         <v>1.1796381826573901</v>
       </c>
       <c r="D81">
-        <f t="shared" si="4"/>
+        <f>B81+C81</f>
         <v>169.5129715159909</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>165</v>
       </c>
       <c r="B82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>166.66666666666686</v>
       </c>
       <c r="C82" s="2">
         <v>-7.3025164292765199</v>
       </c>
       <c r="D82">
-        <f t="shared" si="4"/>
+        <f>B82+C82</f>
         <v>159.36415023739033</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>167</v>
       </c>
       <c r="B83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>165.0000000000002</v>
       </c>
       <c r="C83" s="2">
         <v>-5.2711792382992302</v>
       </c>
       <c r="D83">
-        <f t="shared" si="4"/>
+        <f>B83+C83</f>
         <v>159.72882076170097</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>169</v>
       </c>
       <c r="B84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>163.33333333333354</v>
       </c>
       <c r="C84" s="2">
         <v>1.6876445989451201</v>
       </c>
       <c r="D84">
-        <f t="shared" si="4"/>
+        <f>B84+C84</f>
         <v>165.02097793227867</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>171</v>
       </c>
       <c r="B85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>161.66666666666688</v>
       </c>
       <c r="C85" s="2">
         <v>-1.08644683998839</v>
       </c>
       <c r="D85">
-        <f t="shared" si="4"/>
+        <f>B85+C85</f>
         <v>160.5802198266785</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>173</v>
       </c>
       <c r="B86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>160.00000000000023</v>
       </c>
       <c r="C86" s="2">
         <v>-5.3873279420063902</v>
       </c>
       <c r="D86">
-        <f t="shared" si="4"/>
+        <f>B86+C86</f>
         <v>154.61267205799385</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>175</v>
       </c>
       <c r="B87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>158.33333333333357</v>
       </c>
       <c r="C87" s="2">
         <v>5.9156602539091097</v>
       </c>
       <c r="D87">
-        <f t="shared" si="4"/>
+        <f>B87+C87</f>
         <v>164.24899358724269</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>177</v>
       </c>
       <c r="B88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>156.66666666666691</v>
       </c>
       <c r="C88" s="2">
         <v>-3.2685752351102102</v>
       </c>
       <c r="D88">
-        <f t="shared" si="4"/>
+        <f>B88+C88</f>
         <v>153.39809143155671</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>179</v>
       </c>
       <c r="B89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>155.00000000000026</v>
       </c>
       <c r="C89" s="2">
         <v>-3.16474552475972</v>
       </c>
       <c r="D89">
-        <f t="shared" si="4"/>
+        <f>B89+C89</f>
         <v>151.83525447524053</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>181</v>
       </c>
       <c r="B90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>153.3333333333336</v>
       </c>
       <c r="C90" s="2">
         <v>2.77266514091664E-3</v>
       </c>
       <c r="D90">
-        <f t="shared" si="4"/>
+        <f>B90+C90</f>
         <v>153.33610599847452</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>183</v>
       </c>
       <c r="B91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>151.66666666666694</v>
       </c>
       <c r="C91" s="2">
         <v>0.91054269789695097</v>
       </c>
       <c r="D91">
-        <f t="shared" si="4"/>
+        <f>B91+C91</f>
         <v>152.57720936456388</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>185</v>
       </c>
@@ -5899,11 +5899,11 @@
         <v>3.27710795456988</v>
       </c>
       <c r="D92">
-        <f t="shared" si="4"/>
+        <f>B92+C92</f>
         <v>153.27710795456989</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>187</v>
       </c>
@@ -5915,459 +5915,459 @@
         <v>10.28065987678</v>
       </c>
       <c r="D93">
-        <f t="shared" si="4"/>
+        <f>B93+C93</f>
         <v>161.94732654344665</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>189</v>
       </c>
       <c r="B94">
-        <f t="shared" ref="B94:B121" si="5">B93+($B$122-$B$92)/30</f>
+        <f t="shared" ref="B94:B121" si="3">B93+($B$122-$B$92)/30</f>
         <v>153.33333333333331</v>
       </c>
       <c r="C94" s="2">
         <v>-7.0537328200908398</v>
       </c>
       <c r="D94">
-        <f t="shared" si="4"/>
+        <f>B94+C94</f>
         <v>146.27960051324249</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>191</v>
       </c>
       <c r="B95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>154.99999999999997</v>
       </c>
       <c r="C95" s="2">
         <v>4.07490783229757</v>
       </c>
       <c r="D95">
-        <f t="shared" si="4"/>
+        <f>B95+C95</f>
         <v>159.07490783229755</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>193</v>
       </c>
       <c r="B96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>156.66666666666663</v>
       </c>
       <c r="C96" s="2">
         <v>5.6662985027571997</v>
       </c>
       <c r="D96">
-        <f t="shared" si="4"/>
+        <f>B96+C96</f>
         <v>162.33296516942383</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>195</v>
       </c>
       <c r="B97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>158.33333333333329</v>
       </c>
       <c r="C97" s="2">
         <v>3.3850156215608602</v>
       </c>
       <c r="D97">
-        <f t="shared" si="4"/>
+        <f>B97+C97</f>
         <v>161.71834895489414</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>197</v>
       </c>
       <c r="B98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>159.99999999999994</v>
       </c>
       <c r="C98" s="2">
         <v>-3.6878842146149902</v>
       </c>
       <c r="D98">
-        <f t="shared" si="4"/>
+        <f>B98+C98</f>
         <v>156.31211578538495</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>199</v>
       </c>
       <c r="B99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>161.6666666666666</v>
       </c>
       <c r="C99" s="2">
         <v>7.6314541650022596</v>
       </c>
       <c r="D99">
-        <f t="shared" si="4"/>
+        <f>B99+C99</f>
         <v>169.29812083166885</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>201</v>
       </c>
       <c r="B100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>163.33333333333326</v>
       </c>
       <c r="C100" s="2">
         <v>-2.5458919562576701</v>
       </c>
       <c r="D100">
-        <f t="shared" si="4"/>
+        <f>B100+C100</f>
         <v>160.7874413770756</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>203</v>
       </c>
       <c r="B101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>164.99999999999991</v>
       </c>
       <c r="C101" s="2">
         <v>1.5500272662919601</v>
       </c>
       <c r="D101">
-        <f t="shared" si="4"/>
+        <f>B101+C101</f>
         <v>166.55002726629186</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>205</v>
       </c>
       <c r="B102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>166.66666666666657</v>
       </c>
       <c r="C102" s="2">
         <v>2.18542171721676</v>
       </c>
       <c r="D102">
-        <f t="shared" si="4"/>
+        <f>B102+C102</f>
         <v>168.85208838388334</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>207</v>
       </c>
       <c r="B103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>168.33333333333323</v>
       </c>
       <c r="C103" s="2">
         <v>3.0515317182666499</v>
       </c>
       <c r="D103">
-        <f t="shared" si="4"/>
+        <f>B103+C103</f>
         <v>171.38486505159989</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>209</v>
       </c>
       <c r="B104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>169.99999999999989</v>
       </c>
       <c r="C104" s="2">
         <v>-4.6901769465627199</v>
       </c>
       <c r="D104">
-        <f t="shared" si="4"/>
+        <f>B104+C104</f>
         <v>165.30982305343716</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>211</v>
       </c>
       <c r="B105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>171.66666666666654</v>
       </c>
       <c r="C105" s="2">
         <v>6.8712395687943797</v>
       </c>
       <c r="D105">
-        <f t="shared" si="4"/>
+        <f>B105+C105</f>
         <v>178.53790623546092</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>213</v>
       </c>
       <c r="B106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>173.3333333333332</v>
       </c>
       <c r="C106" s="2">
         <v>-3.3178107904231502</v>
       </c>
       <c r="D106">
-        <f t="shared" si="4"/>
+        <f>B106+C106</f>
         <v>170.01552254291005</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>215</v>
       </c>
       <c r="B107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>174.99999999999986</v>
       </c>
       <c r="C107" s="2">
         <v>-7.12628944918412</v>
       </c>
       <c r="D107">
-        <f t="shared" si="4"/>
+        <f>B107+C107</f>
         <v>167.87371055081573</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>217</v>
       </c>
       <c r="B108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>176.66666666666652</v>
       </c>
       <c r="C108" s="2">
         <v>7.7185126986440604</v>
       </c>
       <c r="D108">
-        <f t="shared" si="4"/>
+        <f>B108+C108</f>
         <v>184.38517936531056</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>219</v>
       </c>
       <c r="B109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>178.33333333333317</v>
       </c>
       <c r="C109" s="2">
         <v>-2.27009990640224</v>
       </c>
       <c r="D109">
-        <f t="shared" si="4"/>
+        <f>B109+C109</f>
         <v>176.06323342693094</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>221</v>
       </c>
       <c r="B110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>179.99999999999983</v>
       </c>
       <c r="C110" s="2">
         <v>-3.6053531401332699</v>
       </c>
       <c r="D110">
-        <f t="shared" si="4"/>
+        <f>B110+C110</f>
         <v>176.39464685986655</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>223</v>
       </c>
       <c r="B111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>181.66666666666649</v>
       </c>
       <c r="C111" s="2">
         <v>-3.1461623236974101</v>
       </c>
       <c r="D111">
-        <f t="shared" si="4"/>
+        <f>B111+C111</f>
         <v>178.52050434296908</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>225</v>
       </c>
       <c r="B112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>183.33333333333314</v>
       </c>
       <c r="C112" s="2">
         <v>2.7789145378898499</v>
       </c>
       <c r="D112">
-        <f t="shared" si="4"/>
+        <f>B112+C112</f>
         <v>186.11224787122299</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>227</v>
       </c>
       <c r="B113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>184.9999999999998</v>
       </c>
       <c r="C113" s="2">
         <v>-2.8559467539757302</v>
       </c>
       <c r="D113">
-        <f t="shared" si="4"/>
+        <f>B113+C113</f>
         <v>182.14405324602407</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>229</v>
       </c>
       <c r="B114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>186.66666666666646</v>
       </c>
       <c r="C114" s="2">
         <v>7.1575236307074199</v>
       </c>
       <c r="D114">
-        <f t="shared" si="4"/>
+        <f>B114+C114</f>
         <v>193.82419029737389</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>231</v>
       </c>
       <c r="B115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>188.33333333333312</v>
       </c>
       <c r="C115" s="2">
         <v>-10.831107805821301</v>
       </c>
       <c r="D115">
-        <f t="shared" si="4"/>
+        <f>B115+C115</f>
         <v>177.50222552751183</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>233</v>
       </c>
       <c r="B116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>189.99999999999977</v>
       </c>
       <c r="C116" s="2">
         <v>2.27844977380997</v>
       </c>
       <c r="D116">
-        <f t="shared" si="4"/>
+        <f>B116+C116</f>
         <v>192.27844977380974</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>235</v>
       </c>
       <c r="B117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>191.66666666666643</v>
       </c>
       <c r="C117" s="2">
         <v>-5.4275916121480403</v>
       </c>
       <c r="D117">
-        <f t="shared" si="4"/>
+        <f>B117+C117</f>
         <v>186.23907505451839</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>237</v>
       </c>
       <c r="B118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>193.33333333333309</v>
       </c>
       <c r="C118" s="2">
         <v>-8.3952882846168801</v>
       </c>
       <c r="D118">
-        <f t="shared" si="4"/>
+        <f>B118+C118</f>
         <v>184.93804504871622</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>239</v>
       </c>
       <c r="B119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>194.99999999999974</v>
       </c>
       <c r="C119" s="2">
         <v>-16.235225410940998</v>
       </c>
       <c r="D119">
-        <f t="shared" si="4"/>
+        <f>B119+C119</f>
         <v>178.76477458905873</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>241</v>
       </c>
       <c r="B120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>196.6666666666664</v>
       </c>
       <c r="C120" s="2">
         <v>-6.8531138999806496</v>
       </c>
       <c r="D120">
-        <f t="shared" si="4"/>
+        <f>B120+C120</f>
         <v>189.81355276668575</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>243</v>
       </c>
       <c r="B121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>198.33333333333306</v>
       </c>
       <c r="C121" s="2">
         <v>-2.9626354950363099</v>
       </c>
       <c r="D121">
-        <f t="shared" si="4"/>
+        <f>B121+C121</f>
         <v>195.37069783829673</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>245</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>200</v>
       </c>
       <c r="D122">
-        <f t="shared" si="4"/>
+        <f>B122+C122</f>
         <v>200</v>
       </c>
     </row>
@@ -6394,12 +6394,12 @@
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>103.93550071329705</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>6.9444444444444447E-4</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>112.6273929606576</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.3888888888888889E-3</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>101.10580541063953</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2.0833333333333298E-3</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>106.91001992018219</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2.7777777777777801E-3</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>121.07217741589041</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3.4722222222222199E-3</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>111.30738183959876</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4.1666666666666701E-3</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>114.58592503686488</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>4.8611111111111103E-3</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>115.23896413109017</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>5.5555555555555601E-3</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>131.4096475083129</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>6.2500000000000003E-3</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>122.17435564301495</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6.9444444444444397E-3</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>135.79802805405936</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7.6388888888888904E-3</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>133.87564868364132</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8.3333333333333297E-3</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>145.59103255259427</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>9.0277777777777804E-3</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>159.60010257357604</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>9.7222222222222206E-3</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>139.20965488522441</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1.0416666666666701E-2</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>146.34332878040587</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1.1111111111111099E-2</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>148.84544162720573</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1.18055555555556E-2</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>148.63930239604326</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>162.47213682962263</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>1.3194444444444399E-2</v>
       </c>
@@ -6567,7 +6567,7 @@
         <v>167.9902643783058</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1.38888888888889E-2</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>163.66890364036109</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1.4583333333333301E-2</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>170.45596881431027</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1.52777777777778E-2</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>172.31726313277488</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1.59722222222222E-2</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>179.38141588640545</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>1.6666666666666701E-2</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>175.82275906584638</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1.7361111111111101E-2</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>192.90443333081663</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1.8055555555555599E-2</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>192.18645875804674</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>193.20911325018139</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>1.94444444444444E-2</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>190.48038599481865</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2.0138888888888901E-2</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>204.81783883861806</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2.0833333333333301E-2</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>193.64820543994799</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2.1527777777777798E-2</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>195.37622365203055</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2.2222222222222199E-2</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>195.2055972460029</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2.29166666666667E-2</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>201.2111766150156</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2.36111111111111E-2</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>195.21709035466213</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2.4305555555555601E-2</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>202.39145236007519</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>195.21423465395529</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2.5694444444444402E-2</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>200.77219147691684</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>2.6388888888888899E-2</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>198.02670582080722</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2.70833333333333E-2</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>196.89952092431022</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>2.7777777777777801E-2</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>203.60989863963673</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2.8472222222222201E-2</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>195.21886273640112</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>2.9166666666666698E-2</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>196.88805245844452</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>2.9861111111111099E-2</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>199.94114015116378</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>3.05555555555556E-2</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>210.09841760005031</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>3.125E-2</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>207.48244756170888</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>3.19444444444444E-2</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>200.49883097426724</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3.2638888888888898E-2</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>201.50902649532341</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>3.3333333333333298E-2</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>204.14343912819092</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3.4027777777777803E-2</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>198.29572478872768</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3.4722222222222203E-2</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>204.46315038332912</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3.54166666666667E-2</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>199.2329877844746</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>3.6111111111111101E-2</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>201.51826884997189</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>3.6805555555555598E-2</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>197.33249405124982</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>202.40333221856304</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>3.8194444444444399E-2</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>189.202459949858</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>3.8888888888888903E-2</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>198.87273464612576</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>3.9583333333333297E-2</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>202.24324692124225</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>4.0277777777777801E-2</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>202.62171606787652</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4.0972222222222202E-2</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>205.19038281758338</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>204.54852512541262</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>4.2361111111111099E-2</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>201.03669346561861</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>4.3055555555555597E-2</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>192.82729187084263</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>4.3749999999999997E-2</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>194.04827187841636</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>4.4444444444444398E-2</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>193.87694076952852</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>4.5138888888888902E-2</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>193.29194626290874</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>4.5833333333333302E-2</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>186.12181537587148</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>4.65277777777778E-2</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>181.88980736671616</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>4.72222222222222E-2</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>189.44183667729342</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>4.7916666666666698E-2</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>179.85299052302983</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>4.8611111111111098E-2</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>190.71580192655315</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>4.9305555555555602E-2</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>190.4714500928678</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>0.05</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>175.87806447442546</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>5.0694444444444403E-2</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>177.80872245267145</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>5.1388888888888901E-2</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>174.47941829661187</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>5.2083333333333301E-2</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>175.05619914284975</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>5.2777777777777798E-2</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>176.96196334923121</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>5.3472222222222199E-2</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>169.20543021485616</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>5.4166666666666703E-2</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>179.04956156266439</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>5.4861111111111097E-2</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>169.5129715159909</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>5.5555555555555601E-2</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>159.36415023739033</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>159.72882076170097</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>5.6944444444444402E-2</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>165.02097793227867</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>5.7638888888888899E-2</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>160.5802198266785</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>5.83333333333333E-2</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>154.61267205799385</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>5.9027777777777797E-2</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>164.24899358724269</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>5.9722222222222197E-2</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>153.39809143155671</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>6.0416666666666702E-2</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>151.83525447524053</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>6.1111111111111102E-2</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>153.33610599847452</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>6.18055555555556E-2</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>152.57720936456388</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>6.25E-2</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>153.27710795456989</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>6.31944444444444E-2</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>161.94732654344665</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>6.3888888888888898E-2</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>146.27960051324249</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>6.4583333333333298E-2</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>159.07490783229755</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>6.5277777777777796E-2</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>162.33296516942383</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>6.5972222222222196E-2</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>161.71834895489414</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>6.6666666666666693E-2</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>156.31211578538495</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>6.7361111111111094E-2</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>169.29812083166885</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>6.8055555555555605E-2</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>160.7874413770756</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>6.8750000000000006E-2</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>166.55002726629186</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>6.9444444444444406E-2</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>168.85208838388334</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>7.0138888888888903E-2</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>171.38486505159989</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>7.0833333333333304E-2</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>165.30982305343716</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>7.1527777777777801E-2</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>178.53790623546092</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>7.2222222222222202E-2</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>170.01552254291005</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>7.2916666666666699E-2</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>167.87371055081573</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>7.3611111111111099E-2</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>184.38517936531056</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>7.4305555555555597E-2</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>176.06323342693094</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>176.39464685986655</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>7.5694444444444495E-2</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>178.52050434296908</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>7.6388888888888895E-2</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>186.11224787122299</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>7.7083333333333295E-2</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>182.14405324602407</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>7.7777777777777807E-2</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>193.82419029737389</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>7.8472222222222193E-2</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>177.50222552751183</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>7.9166666666666705E-2</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>192.27844977380974</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>7.9861111111111105E-2</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>186.23907505451839</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>8.0555555555555602E-2</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>184.93804504871622</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>178.76477458905873</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>8.1944444444444403E-2</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>189.81355276668575</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>8.2638888888888901E-2</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>195.37069783829673</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>8.3333333333333301E-2</v>
       </c>

</xml_diff>